<commit_message>
Update in the sprint
</commit_message>
<xml_diff>
--- a/sprint/tracking_sheet.xlsx
+++ b/sprint/tracking_sheet.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksumanth\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09C1F2E3-256B-44A3-B214-AC4ECFB051B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>DATE</t>
   </si>
@@ -109,13 +103,16 @@
   </si>
   <si>
     <t>over due</t>
+  </si>
+  <si>
+    <t>1) find the best service providers suitable to our project like aws etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -272,7 +269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -449,33 +446,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -511,11 +508,14 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -526,7 +526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -537,7 +537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -548,7 +548,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -559,7 +559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -570,7 +570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -581,7 +581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -592,22 +592,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="4"/>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:6">
       <c r="E22" s="3"/>
       <c r="F22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:6">
       <c r="E23" s="2"/>
       <c r="F23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:6">
       <c r="E24" s="5"/>
       <c r="F24" t="s">
         <v>27</v>

</xml_diff>